<commit_message>
merge reese's REALLY weird, very bad worst practices -100/100 data file
</commit_message>
<xml_diff>
--- a/data/data_file.xlsx
+++ b/data/data_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>oppID</t>
   </si>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t>OPE-0002935252</t>
+  </si>
+  <si>
+    <t>ExcelSheet</t>
+  </si>
+  <si>
+    <t>DESSTEPS_338039_HPFS QUOTE Products.xlsx</t>
+  </si>
+  <si>
+    <t>TargetPrice</t>
+  </si>
+  <si>
+    <t>ExternalComment</t>
+  </si>
+  <si>
+    <t>HPFS Quote</t>
+  </si>
+  <si>
+    <t>OutputType</t>
+  </si>
+  <si>
+    <t>No list or extended list displayed. Line item descriptions with estimated delivery only and Grand Total</t>
+  </si>
+  <si>
+    <t>Test Quote</t>
   </si>
   <si>
     <t>CustomImagingNumber</t>
@@ -440,108 +464,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" customWidth="1"/>
+    <col min="1" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
       </c>
       <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="N2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" t="s">
-        <v>25</v>
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging over fixed code
</commit_message>
<xml_diff>
--- a/data/data_file.xlsx
+++ b/data/data_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>oppID</t>
   </si>
@@ -110,6 +110,30 @@
   </si>
   <si>
     <t>apassword</t>
+  </si>
+  <si>
+    <t>CustomImagingNumber</t>
+  </si>
+  <si>
+    <t>AssetTaggingNumber</t>
+  </si>
+  <si>
+    <t>HA842A1</t>
+  </si>
+  <si>
+    <t>HA841A1</t>
+  </si>
+  <si>
+    <t>ThirdPartyNumber</t>
+  </si>
+  <si>
+    <t>CustomPackingNumber</t>
+  </si>
+  <si>
+    <t>HA844A1</t>
+  </si>
+  <si>
+    <t>ZU706A</t>
   </si>
 </sst>
 </file>
@@ -458,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +502,7 @@
     <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,47 +515,59 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -545,42 +581,54 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="L2">
+      <c r="P2">
         <v>100</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added login function to US9411_02
</commit_message>
<xml_diff>
--- a/data/data_file.xlsx
+++ b/data/data_file.xlsx
@@ -106,12 +106,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>apassword</t>
-  </si>
-  <si>
     <t>CustomImagingNumber</t>
   </si>
   <si>
@@ -134,13 +128,19 @@
   </si>
   <si>
     <t>ZU706A</t>
+  </si>
+  <si>
+    <t>taousautotester@hpe.com</t>
+  </si>
+  <si>
+    <t>5810ca086fd249fe54f03436d5829007179d176ceef6d120c899</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +150,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,14 +180,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -484,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,16 +527,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -581,16 +592,16 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
         <v>6</v>
@@ -625,15 +636,18 @@
       <c r="S2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>30</v>
+      <c r="T2" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="T2" r:id="rId1" display="mailto:taousautotester@hpe.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>